<commit_message>
Added Graphs + edited data
</commit_message>
<xml_diff>
--- a/000_basics/AircraftADSBData.xlsx
+++ b/000_basics/AircraftADSBData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\Documents\SourceCode\DATA_SCIENCE\ai_and_data_repo_0001\000_basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826021FA-988F-41D7-B10B-D589F09F9772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F2D532-034A-46F9-9C05-88D0B3F4CA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="22215" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22050" yWindow="2340" windowWidth="16170" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +463,7 @@
         <v>-77.05</v>
       </c>
       <c r="F2" s="2">
-        <v>32000</v>
+        <v>30000</v>
       </c>
       <c r="G2" s="2">
         <v>460</v>
@@ -515,7 +515,7 @@
         <v>-77.45</v>
       </c>
       <c r="F4" s="2">
-        <v>33000</v>
+        <v>30000</v>
       </c>
       <c r="G4" s="2">
         <v>470</v>

</xml_diff>

<commit_message>
Data edits + file renames
</commit_message>
<xml_diff>
--- a/000_basics/AircraftADSBData.xlsx
+++ b/000_basics/AircraftADSBData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\Documents\SourceCode\DATA_SCIENCE\ai_and_data_repo_0001\000_basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F2D532-034A-46F9-9C05-88D0B3F4CA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E2865A-2B2E-4870-A52D-27F23659F127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22050" yWindow="2340" windowWidth="16170" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4545" yWindow="210" windowWidth="21060" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -410,7 +410,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
         <v>-76.900000000000006</v>
       </c>
       <c r="F7" s="2">
-        <v>28000</v>
+        <v>27500</v>
       </c>
       <c r="G7" s="2">
         <v>430</v>

</xml_diff>

<commit_message>
Added notebook for the same data
</commit_message>
<xml_diff>
--- a/000_basics/AircraftADSBData.xlsx
+++ b/000_basics/AircraftADSBData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\Documents\SourceCode\DATA_SCIENCE\ai_and_data_repo_0001\000_basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E2865A-2B2E-4870-A52D-27F23659F127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EFFF11-1007-4CAF-AE52-4C9CF8658516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4545" yWindow="210" windowWidth="21060" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>